<commit_message>
Finished the Gantt Chart
</commit_message>
<xml_diff>
--- a/planning/Gantt Chart.xlsx
+++ b/planning/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210473BB-8887-435B-94B4-377A900A3CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32488402-9845-4CCA-8AC9-1F525B9FCF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1391,6 +1391,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1408,15 +1417,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2029,7 +2029,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2079,137 +2079,137 @@
       <c r="B3" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93">
+      <c r="D3" s="95"/>
+      <c r="E3" s="96">
         <f>DATE(2025,11,11)</f>
         <v>45972</v>
       </c>
-      <c r="F3" s="93"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="91">
         <f>I5</f>
         <v>45964</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="91">
         <f>P5</f>
         <v>45971</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="91">
         <f>W5</f>
         <v>45978</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
         <v>45985</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
         <v>45992</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
         <v>45999</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
         <v>46006</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
         <v>46013</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
-      <c r="BM4" s="88">
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="91">
         <f>BM5</f>
         <v>46020</v>
       </c>
-      <c r="BN4" s="89"/>
-      <c r="BO4" s="89"/>
-      <c r="BP4" s="89"/>
-      <c r="BQ4" s="89"/>
-      <c r="BR4" s="89"/>
-      <c r="BS4" s="90"/>
-      <c r="BT4" s="88">
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="92"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="91">
         <f>BT5</f>
         <v>46027</v>
       </c>
-      <c r="BU4" s="89"/>
-      <c r="BV4" s="89"/>
-      <c r="BW4" s="89"/>
-      <c r="BX4" s="89"/>
-      <c r="BY4" s="89"/>
-      <c r="BZ4" s="90"/>
-      <c r="CA4" s="88">
+      <c r="BU4" s="92"/>
+      <c r="BV4" s="92"/>
+      <c r="BW4" s="92"/>
+      <c r="BX4" s="92"/>
+      <c r="BY4" s="92"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="91">
         <f>CA5</f>
         <v>46034</v>
       </c>
-      <c r="CB4" s="89"/>
-      <c r="CC4" s="89"/>
-      <c r="CD4" s="89"/>
-      <c r="CE4" s="89"/>
-      <c r="CF4" s="89"/>
-      <c r="CG4" s="90"/>
+      <c r="CB4" s="92"/>
+      <c r="CC4" s="92"/>
+      <c r="CD4" s="92"/>
+      <c r="CE4" s="92"/>
+      <c r="CF4" s="92"/>
+      <c r="CG4" s="93"/>
     </row>
     <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
@@ -3034,7 +3034,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="71">
         <f>Project_Start</f>
@@ -3136,7 +3136,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="17">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="71">
         <f>F9</f>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="88" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="52" t="s">
@@ -3329,7 +3329,7 @@
       <c r="A12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="89" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="52" t="s">
@@ -3630,7 +3630,7 @@
     </row>
     <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45"/>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="89" t="s">
         <v>81</v>
       </c>
       <c r="C15" s="52" t="s">
@@ -3926,7 +3926,7 @@
     </row>
     <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="90" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="54" t="s">
@@ -4729,17 +4729,17 @@
         <v>0</v>
       </c>
       <c r="E26" s="77">
-        <f>F24+1</f>
-        <v>45995</v>
+        <f>E25</f>
+        <v>45996</v>
       </c>
       <c r="F26" s="77">
-        <f>E26</f>
-        <v>45995</v>
+        <f>E26+7</f>
+        <v>46003</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
@@ -4829,17 +4829,17 @@
         <v>0</v>
       </c>
       <c r="E27" s="77">
-        <f>F26</f>
-        <v>45995</v>
+        <f>E25</f>
+        <v>45996</v>
       </c>
       <c r="F27" s="77">
-        <f>E27</f>
-        <v>45995</v>
+        <f>E27+14</f>
+        <v>46010</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -4929,17 +4929,17 @@
         <v>0</v>
       </c>
       <c r="E28" s="77">
-        <f>F27</f>
-        <v>45995</v>
+        <f>E25</f>
+        <v>45996</v>
       </c>
       <c r="F28" s="77">
-        <f>E28</f>
-        <v>45995</v>
+        <f>E28+14</f>
+        <v>46010</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -5029,17 +5029,17 @@
         <v>0</v>
       </c>
       <c r="E29" s="77">
-        <f>F28</f>
-        <v>45995</v>
+        <f>F26</f>
+        <v>46003</v>
       </c>
       <c r="F29" s="77">
-        <f>E29</f>
-        <v>45995</v>
+        <f>E29+14</f>
+        <v>46017</v>
       </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -5128,8 +5128,14 @@
       <c r="D30" s="23">
         <v>0</v>
       </c>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
+      <c r="E30" s="77">
+        <f>F27</f>
+        <v>46010</v>
+      </c>
+      <c r="F30" s="77">
+        <f>E30+5</f>
+        <v>46015</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="31"/>
@@ -5221,8 +5227,14 @@
       <c r="D31" s="23">
         <v>0</v>
       </c>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
+      <c r="E31" s="77">
+        <f>F30</f>
+        <v>46015</v>
+      </c>
+      <c r="F31" s="77">
+        <f>E31+3</f>
+        <v>46018</v>
+      </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="31"/>
@@ -5313,17 +5325,17 @@
         <v>0</v>
       </c>
       <c r="E32" s="77">
-        <f>E28</f>
-        <v>45995</v>
+        <f>F27</f>
+        <v>46010</v>
       </c>
       <c r="F32" s="77">
-        <f>E32</f>
-        <v>45995</v>
+        <f>E32+4</f>
+        <v>46014</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
@@ -5412,7 +5424,10 @@
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="25"/>
-      <c r="E33" s="78"/>
+      <c r="E33" s="78">
+        <f>MAX(F26:F32)</f>
+        <v>46018</v>
+      </c>
       <c r="F33" s="79"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14" t="str">
@@ -5507,17 +5522,17 @@
         <v>0</v>
       </c>
       <c r="E34" s="80">
-        <f>F32+1</f>
-        <v>45996</v>
+        <f>E33</f>
+        <v>46018</v>
       </c>
       <c r="F34" s="80">
-        <f t="shared" ref="F34:F39" si="25">E34</f>
-        <v>45996</v>
+        <f>E34+7</f>
+        <v>46025</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
@@ -5607,17 +5622,17 @@
         <v>0</v>
       </c>
       <c r="E35" s="80">
-        <f>F34</f>
-        <v>45996</v>
+        <f>E33</f>
+        <v>46018</v>
       </c>
       <c r="F35" s="80">
-        <f t="shared" si="25"/>
-        <v>45996</v>
+        <f>E35+5</f>
+        <v>46023</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I35" s="31"/>
       <c r="J35" s="31"/>
@@ -5707,17 +5722,17 @@
         <v>0</v>
       </c>
       <c r="E36" s="80">
-        <f>F35</f>
-        <v>45996</v>
+        <f>E34</f>
+        <v>46018</v>
       </c>
       <c r="F36" s="80">
-        <f t="shared" si="25"/>
-        <v>45996</v>
+        <f>F34</f>
+        <v>46025</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I36" s="31"/>
       <c r="J36" s="31"/>
@@ -5807,17 +5822,17 @@
         <v>0</v>
       </c>
       <c r="E37" s="80">
-        <f>F36</f>
-        <v>45996</v>
+        <f>E16</f>
+        <v>45986</v>
       </c>
       <c r="F37" s="80">
-        <f t="shared" si="25"/>
-        <v>45996</v>
+        <f>E37+28</f>
+        <v>46014</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="31"/>
@@ -5907,17 +5922,17 @@
         <v>0</v>
       </c>
       <c r="E38" s="80">
-        <f>F37</f>
-        <v>45996</v>
+        <f>E36</f>
+        <v>46018</v>
       </c>
       <c r="F38" s="80">
-        <f t="shared" si="25"/>
-        <v>45996</v>
+        <f>F36-14</f>
+        <v>46011</v>
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="14">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="I38" s="31"/>
       <c r="J38" s="31"/>
@@ -6007,12 +6022,12 @@
         <v>0</v>
       </c>
       <c r="E39" s="80">
-        <f>DATE(2026,1,6)</f>
-        <v>46028</v>
+        <f>DATE(2026,1,6)-14</f>
+        <v>46014</v>
       </c>
       <c r="F39" s="80">
-        <f t="shared" si="25"/>
-        <v>46028</v>
+        <f>DATE(2026,1,5)</f>
+        <v>46027</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
@@ -6418,7 +6433,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL7 BM5:CG6 I8:CG42">
+  <conditionalFormatting sqref="I5:BL7 I8:CG42 BM5:CG6">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
@@ -6583,6 +6598,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6870,26 +6905,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
@@ -6899,6 +6914,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6917,16 +6944,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>